<commit_message>
R code + CSV REL_APA
</commit_message>
<xml_diff>
--- a/Rstudio/species_by_cluster.xlsx
+++ b/Rstudio/species_by_cluster.xlsx
@@ -498,7 +498,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.1842105263157895</v>
+        <v>0.1983471074380164</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -527,28 +527,28 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>0.3513513513513514</v>
+        <v>0.368421052631579</v>
       </c>
       <c r="D5">
-        <v>0.02702702702702704</v>
+        <v>0.02631578947368422</v>
       </c>
       <c r="E5">
-        <v>0.02702702702702705</v>
+        <v>0.02631578947368423</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0.02702702702702705</v>
+        <v>0.02631578947368423</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
       <c r="I5">
-        <v>0.1891891891891891</v>
+        <v>0.1842105263157895</v>
       </c>
       <c r="J5">
-        <v>0.2162162162162162</v>
+        <v>0.2105263157894737</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -559,19 +559,19 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.038961038961039</v>
+        <v>0.03749999999999996</v>
       </c>
       <c r="C6">
-        <v>0.03896103896103897</v>
+        <v>0.03749999999999999</v>
       </c>
       <c r="D6">
-        <v>0.07792207792207802</v>
+        <v>0.1000000000000001</v>
       </c>
       <c r="E6">
-        <v>0.1168831168831168</v>
+        <v>0.1125</v>
       </c>
       <c r="F6">
-        <v>0.1818181818181819</v>
+        <v>0.1875</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -580,10 +580,10 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>0.1688311688311689</v>
+        <v>0.1625</v>
       </c>
       <c r="J6">
-        <v>0.05194805194805194</v>
+        <v>0.04999999999999998</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -673,7 +673,7 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0.4210526315789473</v>
+        <v>0.4358974358974359</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -688,10 +688,10 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>0.1052631578947369</v>
+        <v>0.1025641025641025</v>
       </c>
       <c r="K9">
-        <v>0.05263157894736845</v>
+        <v>0.05128205128205127</v>
       </c>
     </row>
     <row r="10">
@@ -720,10 +720,10 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0.0961538461538461</v>
+        <v>0.1090909090909091</v>
       </c>
       <c r="J10">
-        <v>0.25</v>
+        <v>0.2363636363636364</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -737,7 +737,7 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>0.3636363636363636</v>
+        <v>0.3714285714285714</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -758,7 +758,7 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>0.03030303030303032</v>
+        <v>0.02857142857142857</v>
       </c>
       <c r="K11">
         <v>0</v>

</xml_diff>